<commit_message>
Dispatcher completed and tested
</commit_message>
<xml_diff>
--- a/Data/Loan Data.xlsx
+++ b/Data/Loan Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b37a6f4f91240ce/UiPath Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPath\Dispatcher_UIBankLoanRequests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_F25DC773A252ABDACC104897819A42245BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE06D3C7-248C-487F-BB96-49C91FC46ABC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6275A0-660C-4F07-A6C9-36F1C182DDBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
     <t>Loan Term</t>
   </si>
   <si>
-    <t>Current Yearly Income</t>
+    <t>Yearly Income</t>
   </si>
   <si>
     <t>Age</t>
@@ -72,11 +72,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,84 +357,84 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2">
+        <v>50000</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
         <v>10000</v>
       </c>
-      <c r="B2" s="1">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1">
-        <v>50000</v>
-      </c>
-      <c r="D2" s="1">
-        <v>32</v>
+      <c r="D2">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>52000</v>
-      </c>
-      <c r="B3" s="1">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>60000</v>
-      </c>
-      <c r="D3" s="1">
-        <v>23</v>
+      <c r="A3">
+        <v>3000</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>20000</v>
+      </c>
+      <c r="D3">
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>750000</v>
-      </c>
-      <c r="B4" s="1">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1">
-        <v>640000</v>
-      </c>
-      <c r="D4" s="1">
-        <v>52</v>
+      <c r="A4">
+        <v>450000</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>700000</v>
+      </c>
+      <c r="D4">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>90000</v>
       </c>
-      <c r="B5" s="1">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1">
-        <v>300000</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>130000</v>
+      </c>
+      <c r="D5">
         <v>45</v>
       </c>
     </row>

</xml_diff>